<commit_message>
Finished, added process bar, cleared prints
</commit_message>
<xml_diff>
--- a/Example/Filled/AR1 - Q1.2023.xlsx
+++ b/Example/Filled/AR1 - Q1.2023.xlsx
@@ -2139,7 +2139,7 @@
         </is>
       </c>
       <c r="F14" s="136" t="n">
-        <v>4168</v>
+        <v>4169</v>
       </c>
       <c r="G14" s="136" t="n">
         <v>0</v>
@@ -2272,7 +2272,7 @@
         </is>
       </c>
       <c r="F19" s="136" t="n">
-        <v>4631</v>
+        <v>4632</v>
       </c>
       <c r="G19" s="136" t="n">
         <v>0</v>
@@ -2347,7 +2347,7 @@
         </is>
       </c>
       <c r="F22" s="136" t="n">
-        <v>2197</v>
+        <v>2201</v>
       </c>
       <c r="G22" s="136" t="n">
         <v>0</v>
@@ -14202,7 +14202,7 @@
         <v>12981.17</v>
       </c>
       <c r="F10" s="141" t="n">
-        <v>916.5700000000001</v>
+        <v>916.5699999999999</v>
       </c>
       <c r="G10" s="143" t="n">
         <v>91970.60000000001</v>
@@ -14239,7 +14239,7 @@
         <v>12981.17</v>
       </c>
       <c r="F11" s="141" t="n">
-        <v>916.5700000000001</v>
+        <v>916.5699999999999</v>
       </c>
       <c r="G11" s="143" t="n">
         <v>91970.60000000001</v>
@@ -14276,7 +14276,7 @@
         <v>12935.17</v>
       </c>
       <c r="F12" s="142" t="n">
-        <v>897.5700000000001</v>
+        <v>897.5699999999999</v>
       </c>
       <c r="G12" s="144" t="n">
         <v>23</v>

</xml_diff>